<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 16:13:06
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,8 +501,10 @@
           <t>BSO</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>45223</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-10-24 00:00:00</t>
+        </is>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -543,8 +541,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>45034</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2023-04-18 00:00:00</t>
+        </is>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -581,8 +581,10 @@
           <t>BSO</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>45355</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-03-04 00:00:00</t>
+        </is>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -619,8 +621,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>45526</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-08-22 00:00:00</t>
+        </is>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -657,8 +661,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>45544</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-09-09 00:00:00</t>
+        </is>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -695,8 +701,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D7" s="2" t="n">
-        <v>44972</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2023-02-15 00:00:00</t>
+        </is>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -733,8 +741,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>45042</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023-04-26 00:00:00</t>
+        </is>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -771,8 +781,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>45076</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2023-05-30 00:00:00</t>
+        </is>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -809,8 +821,10 @@
           <t>BSO</t>
         </is>
       </c>
-      <c r="D10" s="2" t="n">
-        <v>45127</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-07-20 00:00:00</t>
+        </is>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -847,8 +861,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>45170</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-09-01 00:00:00</t>
+        </is>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -885,8 +901,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D12" s="2" t="n">
-        <v>45138</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2023-07-31 00:00:00</t>
+        </is>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -923,8 +941,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D13" s="2" t="n">
-        <v>45149</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023-08-11 00:00:00</t>
+        </is>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -961,8 +981,10 @@
           <t>BSO</t>
         </is>
       </c>
-      <c r="D14" s="2" t="n">
-        <v>45169</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2023-08-31 00:00:00</t>
+        </is>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -999,8 +1021,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>45162</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2023-08-24 00:00:00</t>
+        </is>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1037,8 +1061,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D16" s="2" t="n">
-        <v>45182</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2023-09-13 00:00:00</t>
+        </is>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1075,8 +1101,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>45230</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2023-10-31 00:00:00</t>
+        </is>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1113,8 +1141,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D18" s="2" t="n">
-        <v>45268</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2023-12-08 00:00:00</t>
+        </is>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1151,8 +1181,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D19" s="2" t="n">
-        <v>45316</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2024-01-25 00:00:00</t>
+        </is>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1189,8 +1221,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D20" s="2" t="n">
-        <v>45536</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2024-09-01 00:00:00</t>
+        </is>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1227,8 +1261,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D21" s="2" t="n">
-        <v>45321</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2024-01-30 00:00:00</t>
+        </is>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1265,8 +1301,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D22" s="2" t="n">
-        <v>45316</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2024-01-25 00:00:00</t>
+        </is>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1303,8 +1341,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D23" s="2" t="n">
-        <v>45334</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2024-02-12 00:00:00</t>
+        </is>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1341,8 +1381,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D24" s="2" t="n">
-        <v>45308</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2024-01-17 00:00:00</t>
+        </is>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1379,8 +1421,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D25" s="2" t="n">
-        <v>45344</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2024-02-22 00:00:00</t>
+        </is>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1417,8 +1461,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D26" s="2" t="n">
-        <v>45336</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2024-02-14 00:00:00</t>
+        </is>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1455,8 +1501,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D27" s="2" t="n">
-        <v>45336</v>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2024-02-14 00:00:00</t>
+        </is>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -1493,8 +1541,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D28" s="2" t="n">
-        <v>45336</v>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2024-02-14 00:00:00</t>
+        </is>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1531,8 +1581,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D29" s="2" t="n">
-        <v>45336</v>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2024-02-14 00:00:00</t>
+        </is>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1569,8 +1621,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D30" s="2" t="n">
-        <v>45392</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2024-04-10 00:00:00</t>
+        </is>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -1607,8 +1661,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D31" s="2" t="n">
-        <v>45364</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2024-03-13 00:00:00</t>
+        </is>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1645,8 +1701,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D32" s="2" t="n">
-        <v>45393</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2024-04-11 00:00:00</t>
+        </is>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1683,8 +1741,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D33" s="2" t="n">
-        <v>45397</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2024-04-15 00:00:00</t>
+        </is>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1721,8 +1781,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D34" s="2" t="n">
-        <v>45366</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2024-03-15 00:00:00</t>
+        </is>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -1759,8 +1821,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D35" s="2" t="n">
-        <v>45442</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2024-05-30 00:00:00</t>
+        </is>
       </c>
       <c r="E35" t="n">
         <v>1</v>
@@ -1797,8 +1861,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D36" s="2" t="n">
-        <v>45411</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2024-04-29 00:00:00</t>
+        </is>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1835,8 +1901,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D37" s="2" t="n">
-        <v>45411</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2024-04-29 00:00:00</t>
+        </is>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1873,8 +1941,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D38" s="2" t="n">
-        <v>45463</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2024-06-20 00:00:00</t>
+        </is>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1911,8 +1981,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D39" s="2" t="n">
-        <v>45426</v>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2024-05-14 00:00:00</t>
+        </is>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1949,8 +2021,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D40" s="2" t="n">
-        <v>45426</v>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2024-05-14 00:00:00</t>
+        </is>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -1987,8 +2061,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D41" s="2" t="n">
-        <v>45478</v>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2024-07-05 00:00:00</t>
+        </is>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -2025,8 +2101,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D42" s="2" t="n">
-        <v>45454</v>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2024-06-11 00:00:00</t>
+        </is>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -2063,8 +2141,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D43" s="2" t="n">
-        <v>45454</v>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2024-06-11 00:00:00</t>
+        </is>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -2101,8 +2181,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D44" s="2" t="n">
-        <v>45457</v>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2024-06-14 00:00:00</t>
+        </is>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -2139,8 +2221,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D45" s="2" t="n">
-        <v>45512</v>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2024-08-08 00:00:00</t>
+        </is>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -2177,8 +2261,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D46" s="2" t="n">
-        <v>45474</v>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2024-07-01 00:00:00</t>
+        </is>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -2215,8 +2301,10 @@
           <t>BSO</t>
         </is>
       </c>
-      <c r="D47" s="2" t="n">
-        <v>45485</v>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2024-07-12 00:00:00</t>
+        </is>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -2253,8 +2341,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D48" s="2" t="n">
-        <v>45484</v>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:00:00</t>
+        </is>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -2291,8 +2381,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D49" s="2" t="n">
-        <v>45531</v>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2024-08-27 00:00:00</t>
+        </is>
       </c>
       <c r="E49" t="n">
         <v>1</v>
@@ -2329,8 +2421,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D50" s="2" t="n">
-        <v>45474</v>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2024-07-01 00:00:00</t>
+        </is>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -2367,8 +2461,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D51" s="2" t="n">
-        <v>45531</v>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2024-08-27 00:00:00</t>
+        </is>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -2405,8 +2501,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D52" s="2" t="n">
-        <v>45526</v>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2024-08-22 00:00:00</t>
+        </is>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -2443,8 +2541,10 @@
           <t>KDV</t>
         </is>
       </c>
-      <c r="D53" s="2" t="n">
-        <v>45524</v>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2024-08-20 00:00:00</t>
+        </is>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -2481,8 +2581,10 @@
           <t>VGO</t>
         </is>
       </c>
-      <c r="D54" s="2" t="n">
-        <v>45161</v>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2023-08-23 00:00:00</t>
+        </is>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -2540,6 +2642,46 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>BSO Partou Camplaan 40</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2019-11-07</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 17:59:40
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2685,6 +2685,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:00:08
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2725,6 +2725,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2023-04-28</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:01:20
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2765,6 +2765,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:01:47
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2805,6 +2805,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:02:05
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2845,6 +2845,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2024-06-24</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:02:23
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2885,6 +2885,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Kindergarden Harderwijk Bazuindreef</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:04:40
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2925,6 +2925,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>CompaNanny Benoordenhout KDV</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:05:44
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2965,6 +2965,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CompaNanny Maanplein B.V.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2023-04-24</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:06:28
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3005,6 +3005,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>CompaNanny Rembrandtlaan</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:06:49
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3045,6 +3045,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Kindergarden Den Haag Bezuidenhoutseweg</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:08:10
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3085,6 +3085,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Kindergarden Delft Hugo de Grootstraat</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2024-02-13</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:08:23
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3125,6 +3125,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Kindergarden Delft Zuid</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2023-12-07</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:08:39
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3165,6 +3165,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Kindergarden Den Haag Bankaplein</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:08:51
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3205,6 +3205,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>BSO Partou Fluitenkruid 10</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2024-03-07</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:09:10
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3245,6 +3245,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2023-03-28</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:09:24
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3285,6 +3285,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Partou De Hoven</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2024-04-08</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:09:37
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3325,6 +3325,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CompaNanny Prinsenhof</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2023-12-14</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:09:52
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3365,6 +3365,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Kindergarden Bussum Kamerlingh Onnesweg</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:10:14
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3405,6 +3405,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Kindergarden Hilversum Johannes Geradtsweg</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2024-03-20</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:10:51
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3445,6 +3445,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Kindergarden Naarden Lambertus Hortensiuslaan</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2024-02-29</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:11:09
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3485,6 +3485,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Kindergarden Bussum Brediusweg</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2024-02-21</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:13:30
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3525,6 +3525,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:13:44
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3565,6 +3565,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2023-08-29</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:15:02
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3605,6 +3605,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>CompaNanny Kleine Drift</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2024-06-19</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:15:19
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3645,6 +3645,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2023-07-18</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:15:42
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3685,6 +3685,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:16:00
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3725,6 +3725,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>1</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:16:19
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3765,6 +3765,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Partou Hetty Blokweg 2</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:16:40
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3805,6 +3805,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>BSO Partou Fluitenkruid 10</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2024-06-25</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:21:38
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3845,6 +3845,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Partou KDV Blaricummerstraat 1A</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2024-08-27</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:21:49
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3885,6 +3885,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>KDV Partou De Groeskant 1</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2024-10-14</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:22:23
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3925,6 +3925,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>CompaNanny Amstelveen KDV</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:22:35
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3965,6 +3965,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Kindergarden Den Haag Bezuidenhoutseweg</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:22:49
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4005,6 +4005,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Kindergarden Delft Reinier de Graaf</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2024-08-26</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-03 18:23:14
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4045,6 +4045,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Kindergarden Den Haag Binckhorstlaan</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2024-02-22</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:19:28
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4085,6 +4085,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>CompaNanny Archipel B.V.</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2024-04-02</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:20:23
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4125,6 +4125,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier KDV</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2023-05-04</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:20:37
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4165,6 +4165,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Kindergarden Delft Buitenhofdreef</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2023-12-07</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:20:53
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4205,6 +4205,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Kindergarden Den Haag Appelgaard</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2024-07-29</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>1</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:21:08
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4245,6 +4245,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Kindergarden Den Haag Eisenhowerlaan</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:21:19
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4285,6 +4285,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Kindergarden Almere Zwitserlandstraat</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2023-11-21</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>1</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:21:39
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4325,6 +4325,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Kindergarden Leiden Raamsteeg</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2023-10-19</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:21:53
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4365,6 +4365,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>CompaNanny Burggravenlaan KDV</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>2023-11-09</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:22:10
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4405,6 +4405,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Partou KDV A.J.W. Vogelaarstraat 22</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2024-04-08</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:22:26
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4445,6 +4445,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>CompaNanny Viandenlaan KDV</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2024-04-22</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:22:38
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4485,6 +4485,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Kindergarden Breda Princenhage</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>BSO</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2024-02-08</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:22:54
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4525,6 +4525,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Kindergarden Breda Zuid</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:23:07
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4565,6 +4565,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Partou KDV Burg. Krijgsmangeerde 43</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2024-01-19</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:23:17
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4605,6 +4605,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Partou KDV Abraham Kuyperpark 171</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:23:29
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4645,6 +4645,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Partou Dunantstraat</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2024-03-19</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" t="n">
+        <v>1</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:23:42
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4685,6 +4685,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Partou Hart van Slangenbeek KDV</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2024-08-01</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:23:53
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4725,6 +4725,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Kindergarden Driebergen Valentijn</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:24:34
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4765,6 +4765,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="n">
+        <v>1</v>
+      </c>
+      <c r="J109" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:24:50
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4805,6 +4805,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Partou KDV Berg en Dalseweg 38</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2024-05-07</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:25:01
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4845,6 +4845,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Kindergarden Baarn Teding van Berkhoutstraat</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2024-08-01</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>1</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="n">
+        <v>0</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:25:13
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4885,6 +4885,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Kindergarden De Meern Spinsterlaan</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2024-03-05</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0</v>
+      </c>
+      <c r="J112" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:25:23
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4925,6 +4925,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Kindergarden Amersfoort Bergstraat</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="n">
+        <v>1</v>
+      </c>
+      <c r="J113" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:25:35
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4965,6 +4965,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Partou KDV Ariaweg 115 (VVE Het Scala)</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="n">
+        <v>0</v>
+      </c>
+      <c r="J114" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:25:50
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5005,6 +5005,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Partou KDV Bolstraat 28A</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2024-04-03</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:26:01
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5045,6 +5045,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>CompaNanny Kralingen</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>2024-04-30</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>1</v>
+      </c>
+      <c r="G116" t="n">
+        <v>1</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:26:15
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5085,6 +5085,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>CompaNanny Oegstgeest</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2024-05-08</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:26:25
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5125,6 +5125,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>KDV Partou Westeinde 94</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" t="n">
+        <v>0</v>
+      </c>
+      <c r="J118" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:26:41
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5165,6 +5165,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>KDV Partou In den Houte</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2024-07-29</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:26:59
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5205,6 +5205,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Kindergarden Capelle Rembrandtsingel</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>2024-06-26</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>1</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:27:12
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5245,6 +5245,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Partou KDV Burgemeester Oudlaan 50</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2024-10-22</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" t="n">
+        <v>0</v>
+      </c>
+      <c r="J121" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:27:23
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5285,6 +5285,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>CompaNanny Lent</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2024-04-24</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0</v>
+      </c>
+      <c r="J122" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:27:36
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5325,6 +5325,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Partou Groote Boel KDV</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" t="n">
+        <v>0</v>
+      </c>
+      <c r="J123" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:27:49
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5365,6 +5365,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>KDV Partou Vliet 2</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2024-07-23</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0</v>
+      </c>
+      <c r="H124" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" t="n">
+        <v>0</v>
+      </c>
+      <c r="J124" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:29:14
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5405,6 +5405,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>CompaNanny Lent</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2024-08-13</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0</v>
+      </c>
+      <c r="G125" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="n">
+        <v>0</v>
+      </c>
+      <c r="J125" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:29:27
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J125"/>
+  <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5445,6 +5445,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Partou KDV Artemisstraat 541</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>0</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0</v>
+      </c>
+      <c r="G126" t="n">
+        <v>0</v>
+      </c>
+      <c r="H126" t="n">
+        <v>0</v>
+      </c>
+      <c r="I126" t="n">
+        <v>0</v>
+      </c>
+      <c r="J126" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:29:38
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:J127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5485,6 +5485,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Kindergarden Houten Tuibrug</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>2024-07-23</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" t="n">
+        <v>1</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="n">
+        <v>1</v>
+      </c>
+      <c r="J127" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:31:08
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5525,6 +5525,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>CompaNanny Statenkwartier BSO</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J128" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:31:21
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5565,6 +5565,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Partou KDV Biltstraat 335</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>0</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:31:31
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J129"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5605,6 +5605,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Partou KDV Bergweg 37d</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2024-08-16</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:31:42
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J130"/>
+  <dimension ref="A1:J131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5645,6 +5645,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Kindergarden Houten Draaibrug</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2024-08-22</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:31:54
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J131"/>
+  <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5685,6 +5685,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>CompaNanny</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>CompaNanny Texelstraat B.V.</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2023-08-29</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>1</v>
+      </c>
+      <c r="G132" t="n">
+        <v>1</v>
+      </c>
+      <c r="H132" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:32:22
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J132"/>
+  <dimension ref="A1:J133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5725,6 +5725,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Partou KDV Acacialaan 18A</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:33:08
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5765,6 +5765,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Partou Amsterdamseweg KDV</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2024-07-23</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0</v>
+      </c>
+      <c r="H134" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" t="n">
+        <v>0</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:33:25
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5805,6 +5805,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>KDV Partou Camplaan 40</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2024-08-27</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0</v>
+      </c>
+      <c r="G135" t="n">
+        <v>1</v>
+      </c>
+      <c r="H135" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:34:03
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5845,6 +5845,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Kindergarden Castricum Kortenaerplantsoen</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>0</v>
+      </c>
+      <c r="F136" t="n">
+        <v>0</v>
+      </c>
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" t="n">
+        <v>0</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:34:20
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J136"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5885,6 +5885,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Kindergarden Haarlem Kennemerplein</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>0</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0</v>
+      </c>
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:34:31
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5925,6 +5925,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Kindergarden Haarlem Koningin Wilhelminalaan</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2024-02-29</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>0</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0</v>
+      </c>
+      <c r="G138" t="n">
+        <v>0</v>
+      </c>
+      <c r="H138" t="n">
+        <v>0</v>
+      </c>
+      <c r="I138" t="n">
+        <v>0</v>
+      </c>
+      <c r="J138" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:34:39
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J138"/>
+  <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5965,6 +5965,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Kindergarden Heemstede Sportparklaan</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2024-01-24</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
+      <c r="H139" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:34:48
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J139"/>
+  <dimension ref="A1:J140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6005,6 +6005,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Kindergarden Hoofddorp Floriande</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2024-04-16</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>0</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:34:59
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6045,6 +6045,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Kindergarden Hoofddorp Julianalaan</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="n">
+        <v>1</v>
+      </c>
+      <c r="H141" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:35:10
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6085,6 +6085,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Kindergarden Hoofddorp Spicalaan</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2024-10-15</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:35:20
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J142"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6125,6 +6125,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Kindergarden Nieuw Vennep Helsinkilaan</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2023-08-28</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>0</v>
+      </c>
+      <c r="F143" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:35:32
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J143"/>
+  <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6165,6 +6165,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Kindergarden</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Kindergarden Amsterdam Villa Vondel</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>0</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0</v>
+      </c>
+      <c r="G144" t="n">
+        <v>1</v>
+      </c>
+      <c r="H144" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:37:40
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J144"/>
+  <dimension ref="A1:J145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6205,6 +6205,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Partou KDV Aan Zee</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>VGO</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>0</v>
+      </c>
+      <c r="F145" t="n">
+        <v>1</v>
+      </c>
+      <c r="G145" t="n">
+        <v>1</v>
+      </c>
+      <c r="H145" t="n">
+        <v>1</v>
+      </c>
+      <c r="I145" t="n">
+        <v>1</v>
+      </c>
+      <c r="J145" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:37:59
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6245,6 +6245,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Partou KDV Alexander Flemingstraat 24</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2024-01-09</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>1</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" t="n">
+        <v>1</v>
+      </c>
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:38:10
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J146"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6285,6 +6285,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Partou KDV Beukenstraat 11</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>0</v>
+      </c>
+      <c r="F147" t="n">
+        <v>0</v>
+      </c>
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Nieuwe data toegevoegd via Streamlit op 2024-12-04 11:38:20
</commit_message>
<xml_diff>
--- a/CompaNanny_Database.xlsx
+++ b/CompaNanny_Database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:J148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6325,6 +6325,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Partou</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Partou KDV Boerhaavelaan 32B</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>KDV</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2024-10-31</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>